<commit_message>
Arreglos menores en visualizacion de saldo y nueva prueba de gestion de menu implementada
</commit_message>
<xml_diff>
--- a/src/test/docs/IS Pruebas Unitarias Sprint 2.xlsx
+++ b/src/test/docs/IS Pruebas Unitarias Sprint 2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="180">
   <si>
     <t>Prueba Unitarias, Equipo 1: Javier García, Angel Bello, Oscar Contreras, Diego Benítez,</t>
   </si>
@@ -321,6 +321,12 @@
     <t>("10 febrero 2026","Compota","frutas", "")</t>
   </si>
   <si>
+    <t>Cupos negativos</t>
+  </si>
+  <si>
+    <t>("10 febrero 2026", "Compota", "frutas", "-5")</t>
+  </si>
+  <si>
     <t>Cadena con solo números</t>
   </si>
   <si>
@@ -379,8 +385,8 @@
   </si>
   <si>
     <t>Los inputs deben ser distintos de null y vacío
-la password debe ser longitud &gt;= 8, password==confirmPassword,  de ser asi retorna 1
-Caso contrario retorna 0</t>
+la password debe ser longitud &gt;= 8, password==confirmPassword,  de ser asi retorna true
+Caso contrario retorna false</t>
   </si>
   <si>
     <t>Boolean (True si todas las entradas son distintas de null y vacío, contraseña.lenght()&gt;= 8 y contraseña==confirmarContraseña, False en caso contrario)</t>
@@ -1945,7 +1951,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="30" t="s">
         <v>94</v>
       </c>
@@ -1953,25 +1959,25 @@
         <v>95</v>
       </c>
       <c r="D18" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="17"/>
+      <c r="B19" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="30" t="s">
+    <row r="20">
+      <c r="A20" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="17"/>
       <c r="B20" s="30" t="s">
         <v>99</v>
       </c>
@@ -1979,42 +1985,54 @@
         <v>100</v>
       </c>
       <c r="D20" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="17"/>
+      <c r="B21" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="30" t="s">
+    <row r="22">
+      <c r="A22" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="17"/>
       <c r="B22" s="30" t="s">
         <v>104</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="33"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="30"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A15:A19"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2037,10 +2055,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -2069,10 +2087,10 @@
     <row r="6">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D6" s="21"/>
     </row>
@@ -2110,14 +2128,14 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
@@ -2148,13 +2166,13 @@
     </row>
     <row r="15">
       <c r="A15" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D15" s="30" t="b">
         <v>0</v>
@@ -2163,10 +2181,10 @@
     <row r="16">
       <c r="A16" s="18"/>
       <c r="B16" s="30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D16" s="30" t="b">
         <v>1</v>
@@ -2175,10 +2193,10 @@
     <row r="17">
       <c r="A17" s="18"/>
       <c r="B17" s="30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D17" s="30" t="b">
         <v>0</v>
@@ -2187,10 +2205,10 @@
     <row r="18">
       <c r="A18" s="17"/>
       <c r="B18" s="30" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D18" s="30" t="b">
         <v>0</v>
@@ -2198,13 +2216,13 @@
     </row>
     <row r="19">
       <c r="A19" s="35" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D19" s="30" t="b">
         <v>0</v>
@@ -2213,10 +2231,10 @@
     <row r="20">
       <c r="A20" s="17"/>
       <c r="B20" s="30" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D20" s="30" t="b">
         <v>1</v>
@@ -2224,13 +2242,13 @@
     </row>
     <row r="21">
       <c r="A21" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D21" s="30" t="b">
         <v>0</v>
@@ -2239,10 +2257,10 @@
     <row r="22">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D22" s="30" t="b">
         <v>1</v>
@@ -2251,10 +2269,10 @@
     <row r="23">
       <c r="A23" s="17"/>
       <c r="B23" s="30" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D23" s="30" t="b">
         <v>0</v>
@@ -2289,10 +2307,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -2320,13 +2338,13 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D6" s="21"/>
     </row>
@@ -2364,16 +2382,16 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12">
@@ -2404,62 +2422,62 @@
     </row>
     <row r="15">
       <c r="A15" s="15" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="17"/>
       <c r="B16" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="17"/>
       <c r="B18" s="30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -2487,13 +2505,13 @@
     </row>
     <row r="28">
       <c r="A28" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D28" s="3"/>
     </row>
@@ -2531,16 +2549,16 @@
     </row>
     <row r="33">
       <c r="A33" s="12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34">
@@ -2571,13 +2589,13 @@
     </row>
     <row r="37">
       <c r="A37" s="15" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D37" s="30" t="b">
         <v>1</v>
@@ -2586,10 +2604,10 @@
     <row r="38">
       <c r="A38" s="17"/>
       <c r="B38" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D38" s="30" t="b">
         <v>1</v>
@@ -2597,13 +2615,13 @@
     </row>
     <row r="39">
       <c r="A39" s="15" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D39" s="36" t="b">
         <v>0</v>
@@ -2612,10 +2630,10 @@
     <row r="40">
       <c r="A40" s="18"/>
       <c r="B40" s="30" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D40" s="36" t="b">
         <v>0</v>
@@ -2627,7 +2645,7 @@
         <v>22</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D41" s="36" t="b">
         <v>0</v>
@@ -2636,10 +2654,10 @@
     <row r="42">
       <c r="A42" s="17"/>
       <c r="B42" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D42" s="36" t="b">
         <v>0</v>

</xml_diff>